<commit_message>
Ajuste de formato importación preguntas, enunciado_2
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/16_formato_cargue_preguntas.xlsx
+++ b/assets/formatos_cargue/16_formato_cargue_preguntas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ele4\assets\formatos_cargue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ele\assets\formatos_cargue\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,8 +22,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Mauricio</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PML:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ID de la lectura asociada a la pregunta.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>cod tema</t>
   </si>
@@ -37,9 +71,6 @@
     <t>orden</t>
   </si>
   <si>
-    <t>enunciado_id</t>
-  </si>
-  <si>
     <t>opcion_a</t>
   </si>
   <si>
@@ -58,14 +89,44 @@
     <t>competencia_id</t>
   </si>
   <si>
-    <t>n9-010555</t>
+    <t>lectura_id</t>
+  </si>
+  <si>
+    <t>enunciado complementario</t>
+  </si>
+  <si>
+    <t>P123</t>
+  </si>
+  <si>
+    <t>Este es el texto de la pregunta</t>
+  </si>
+  <si>
+    <t>Este es un enunciado complementario</t>
+  </si>
+  <si>
+    <t>Opcipon A</t>
+  </si>
+  <si>
+    <t>Opción B</t>
+  </si>
+  <si>
+    <t>Opción C</t>
+  </si>
+  <si>
+    <t>Opción D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>l8-u19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +141,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -426,123 +500,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="3" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2">
         <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-      <c r="K3" s="2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="K4" s="2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
-      <c r="K5" s="2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="K6" s="2">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>